<commit_message>
Included mean in code for all experiments
</commit_message>
<xml_diff>
--- a/Circular/Standard_Deviation Circ.xlsx
+++ b/Circular/Standard_Deviation Circ.xlsx
@@ -460,22 +460,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.003657403793311366</v>
+        <v>0.00365740379331137</v>
       </c>
       <c r="C3" t="n">
-        <v>0.003336912593091473</v>
+        <v>0.00333691259309144</v>
       </c>
       <c r="D3" t="n">
-        <v>0.002947881383821372</v>
+        <v>0.002947881383821377</v>
       </c>
       <c r="E3" t="n">
-        <v>0.002741182500643685</v>
+        <v>0.002741182500643684</v>
       </c>
       <c r="F3" t="n">
-        <v>0.003125487339547781</v>
+        <v>0.003125487339547669</v>
       </c>
       <c r="G3" t="n">
-        <v>0.002584348473167857</v>
+        <v>0.002584348473167832</v>
       </c>
     </row>
     <row r="4">
@@ -485,22 +485,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.004426254425890574</v>
+        <v>0.004426254425890571</v>
       </c>
       <c r="C4" t="n">
-        <v>0.004251520876986325</v>
+        <v>0.004251520876986322</v>
       </c>
       <c r="D4" t="n">
-        <v>0.003163996029644579</v>
+        <v>0.003163996029644509</v>
       </c>
       <c r="E4" t="n">
-        <v>0.004811199661304087</v>
+        <v>0.004811199661304071</v>
       </c>
       <c r="F4" t="n">
-        <v>0.004186718158168615</v>
+        <v>0.004186718158168574</v>
       </c>
       <c r="G4" t="n">
-        <v>0.004102613816328485</v>
+        <v>0.004102613816328628</v>
       </c>
     </row>
     <row r="5">
@@ -510,22 +510,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.004567715441244399</v>
+        <v>0.004567715441244391</v>
       </c>
       <c r="C5" t="n">
-        <v>0.003230849380722437</v>
+        <v>0.003230849380722434</v>
       </c>
       <c r="D5" t="n">
-        <v>0.002794778091767255</v>
+        <v>0.002794778091767261</v>
       </c>
       <c r="E5" t="n">
-        <v>0.004872243837479147</v>
+        <v>0.004872243837479119</v>
       </c>
       <c r="F5" t="n">
-        <v>0.004454878938658642</v>
+        <v>0.004454878938658656</v>
       </c>
       <c r="G5" t="n">
-        <v>0.003617873536707983</v>
+        <v>0.003617873536708047</v>
       </c>
     </row>
   </sheetData>

</xml_diff>